<commit_message>
got all of the code in and have 3 of 5 tests working, still chugging on the others
</commit_message>
<xml_diff>
--- a/Clue Layout.xlsx
+++ b/Clue Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\School\Fall_2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CSCI306\ClueGameDEDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="49">
   <si>
     <t>Pewter City Gym</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>Magmar</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -267,7 +273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -325,17 +331,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -359,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -371,7 +366,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -386,14 +380,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,7 +682,7 @@
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AL5" sqref="AL5"/>
+      <selection activeCell="H1" sqref="H1:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -722,22 +713,22 @@
         <v>16</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>16</v>
@@ -804,23 +795,23 @@
       <c r="G2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>17</v>
+      <c r="H2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>16</v>
@@ -828,28 +819,28 @@
       <c r="O2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" s="13" t="s">
+      <c r="Q2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="12" t="s">
         <v>11</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="13" t="s">
         <v>10</v>
       </c>
       <c r="X2" s="7">
@@ -875,7 +866,7 @@
       <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -887,23 +878,23 @@
       <c r="G3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>17</v>
+      <c r="H3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>16</v>
@@ -914,25 +905,25 @@
       <c r="P3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="U3" s="13" t="s">
+      <c r="Q3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="12" t="s">
         <v>11</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W3" s="14" t="s">
+      <c r="W3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="X3" s="7">
@@ -958,7 +949,7 @@
       <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -967,28 +958,28 @@
       <c r="F4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="12" t="s">
+      <c r="H4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="11" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="10" t="s">
@@ -997,25 +988,25 @@
       <c r="P4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="U4" s="13" t="s">
+      <c r="Q4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="V4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="14" t="s">
+      <c r="W4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="X4" s="7">
@@ -1032,7 +1023,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1050,28 +1041,28 @@
       <c r="F5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="12" t="s">
+      <c r="H5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="11" t="s">
         <v>33</v>
       </c>
       <c r="O5" s="10" t="s">
@@ -1080,25 +1071,25 @@
       <c r="P5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="U5" s="13" t="s">
+      <c r="S5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="V5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="14" t="s">
+      <c r="W5" s="13" t="s">
         <v>10</v>
       </c>
       <c r="X5" s="7">
@@ -1115,7 +1106,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1181,7 +1172,7 @@
       <c r="V6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W6" s="16" t="s">
+      <c r="W6" s="15" t="s">
         <v>30</v>
       </c>
       <c r="X6" s="7">
@@ -1198,7 +1189,7 @@
       </c>
     </row>
     <row r="7" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1264,7 +1255,7 @@
       <c r="V7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W7" s="14" t="s">
+      <c r="W7" s="13" t="s">
         <v>10</v>
       </c>
       <c r="X7" s="7">
@@ -1281,19 +1272,19 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="A8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="10" t="s">
@@ -1335,19 +1326,19 @@
       <c r="R8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="T8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="U8" s="18" t="s">
+      <c r="S8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="T8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="17" t="s">
         <v>12</v>
       </c>
       <c r="V8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W8" s="14" t="s">
+      <c r="W8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="X8" s="7">
@@ -1364,19 +1355,19 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="17" t="s">
+      <c r="A9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="10" t="s">
@@ -1388,25 +1379,25 @@
       <c r="H9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" s="12" t="s">
+      <c r="J9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="11" t="s">
         <v>25</v>
       </c>
       <c r="P9" s="10" t="s">
@@ -1418,19 +1409,19 @@
       <c r="R9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="T9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="U9" s="18" t="s">
+      <c r="S9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="T9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U9" s="17" t="s">
         <v>12</v>
       </c>
       <c r="V9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W9" s="20" t="s">
+      <c r="W9" s="19" t="s">
         <v>16</v>
       </c>
       <c r="X9" s="7">
@@ -1447,19 +1438,19 @@
       </c>
     </row>
     <row r="10" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="17" t="s">
+      <c r="A10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -1468,31 +1459,31 @@
       <c r="G10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="N10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="P10" s="19" t="s">
+      <c r="H10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="18" t="s">
         <v>14</v>
       </c>
       <c r="Q10" s="10" t="s">
@@ -1501,19 +1492,19 @@
       <c r="R10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="T10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="U10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="V10" s="12" t="s">
+      <c r="S10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="T10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="V10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="W10" s="16" t="s">
+      <c r="W10" s="15" t="s">
         <v>28</v>
       </c>
       <c r="X10" s="7">
@@ -1530,19 +1521,19 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="17" t="s">
+      <c r="A11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="10" t="s">
@@ -1551,31 +1542,31 @@
       <c r="G11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="19" t="s">
+      <c r="H11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="18" t="s">
         <v>14</v>
       </c>
       <c r="Q11" s="10" t="s">
@@ -1584,19 +1575,19 @@
       <c r="R11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S11" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="T11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="U11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="V11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="W11" s="22" t="s">
+      <c r="S11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="V11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="W11" s="21" t="s">
         <v>12</v>
       </c>
       <c r="X11" s="7">
@@ -1613,19 +1604,19 @@
       </c>
     </row>
     <row r="12" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="A12" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="10" t="s">
@@ -1634,31 +1625,31 @@
       <c r="G12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="19" t="s">
+      <c r="H12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="18" t="s">
         <v>14</v>
       </c>
       <c r="Q12" s="10" t="s">
@@ -1667,19 +1658,19 @@
       <c r="R12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S12" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="T12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="U12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="V12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="W12" s="22" t="s">
+      <c r="S12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="T12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="V12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="W12" s="21" t="s">
         <v>12</v>
       </c>
       <c r="X12" s="7">
@@ -1687,19 +1678,19 @@
       </c>
     </row>
     <row r="13" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="A13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="10" t="s">
@@ -1708,31 +1699,31 @@
       <c r="G13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="19" t="s">
+      <c r="H13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" s="18" t="s">
         <v>14</v>
       </c>
       <c r="Q13" s="10" t="s">
@@ -1741,19 +1732,19 @@
       <c r="R13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="T13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="U13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="V13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="W13" s="22" t="s">
+      <c r="S13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="T13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="V13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="W13" s="21" t="s">
         <v>12</v>
       </c>
       <c r="X13" s="7">
@@ -1767,19 +1758,19 @@
       </c>
     </row>
     <row r="14" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="A14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="10" t="s">
@@ -1791,25 +1782,25 @@
       <c r="H14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="12" t="s">
+      <c r="J14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="11" t="s">
         <v>25</v>
       </c>
       <c r="P14" s="10" t="s">
@@ -1821,19 +1812,19 @@
       <c r="R14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S14" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="T14" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="U14" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="V14" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="W14" s="16" t="s">
+      <c r="S14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="T14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="V14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="W14" s="15" t="s">
         <v>29</v>
       </c>
       <c r="X14" s="7">
@@ -1847,19 +1838,19 @@
       </c>
     </row>
     <row r="15" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="A15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="10" t="s">
@@ -1913,7 +1904,7 @@
       <c r="V15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W15" s="20" t="s">
+      <c r="W15" s="19" t="s">
         <v>16</v>
       </c>
       <c r="X15" s="7">
@@ -1927,7 +1918,7 @@
       </c>
     </row>
     <row r="16" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -1993,7 +1984,7 @@
       <c r="V16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W16" s="20" t="s">
+      <c r="W16" s="19" t="s">
         <v>16</v>
       </c>
       <c r="X16" s="7">
@@ -2007,7 +1998,7 @@
       </c>
     </row>
     <row r="17" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -2034,10 +2025,10 @@
       <c r="I17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="11" t="s">
         <v>23</v>
       </c>
       <c r="L17" s="10" t="s">
@@ -2064,16 +2055,16 @@
       <c r="S17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="T17" s="12" t="s">
+      <c r="T17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="U17" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="V17" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="W17" s="24" t="s">
+      <c r="U17" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="V17" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="W17" s="23" t="s">
         <v>13</v>
       </c>
       <c r="X17" s="7">
@@ -2087,17 +2078,17 @@
       </c>
     </row>
     <row r="18" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>19</v>
+      <c r="A18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>16</v>
@@ -2108,22 +2099,22 @@
       <c r="G18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="M18" s="27" t="s">
+      <c r="H18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="25" t="s">
         <v>18</v>
       </c>
       <c r="N18" s="10" t="s">
@@ -2144,16 +2135,16 @@
       <c r="S18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="T18" s="12" t="s">
+      <c r="T18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="U18" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="V18" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="W18" s="24" t="s">
+      <c r="U18" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="V18" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="W18" s="23" t="s">
         <v>13</v>
       </c>
       <c r="X18" s="7">
@@ -2167,19 +2158,19 @@
       </c>
     </row>
     <row r="19" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="A19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="10" t="s">
@@ -2188,22 +2179,22 @@
       <c r="G19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="M19" s="27" t="s">
+      <c r="H19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="25" t="s">
         <v>18</v>
       </c>
       <c r="N19" s="10" t="s">
@@ -2215,25 +2206,25 @@
       <c r="P19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="R19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="S19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="T19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="U19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="W19" s="24" t="s">
+      <c r="Q19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="R19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="S19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="T19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="U19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="W19" s="23" t="s">
         <v>13</v>
       </c>
       <c r="X19" s="7">
@@ -2241,19 +2232,19 @@
       </c>
     </row>
     <row r="20" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="A20" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="10" t="s">
@@ -2262,22 +2253,22 @@
       <c r="G20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="L20" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="M20" s="27" t="s">
+      <c r="H20" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="25" t="s">
         <v>18</v>
       </c>
       <c r="N20" s="10" t="s">
@@ -2289,25 +2280,25 @@
       <c r="P20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="R20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="S20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="T20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="U20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="V20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="W20" s="24" t="s">
+      <c r="Q20" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="R20" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="S20" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="T20" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="U20" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="V20" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="W20" s="23" t="s">
         <v>13</v>
       </c>
       <c r="X20" s="7">
@@ -2321,17 +2312,17 @@
       </c>
     </row>
     <row r="21" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>19</v>
+      <c r="A21" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>16</v>
@@ -2342,22 +2333,22 @@
       <c r="G21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="L21" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21" s="27" t="s">
+      <c r="H21" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="25" t="s">
         <v>18</v>
       </c>
       <c r="N21" s="10" t="s">
@@ -2369,25 +2360,25 @@
       <c r="P21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="R21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="S21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="T21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="U21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="V21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" s="24" t="s">
+      <c r="Q21" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="R21" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="S21" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="T21" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="U21" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="V21" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="23" t="s">
         <v>13</v>
       </c>
       <c r="X21" s="7">
@@ -2401,73 +2392,73 @@
       </c>
     </row>
     <row r="22" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="M22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="N22" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="P22" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="R22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="S22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="T22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="U22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="V22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="W22" s="33" t="s">
+      <c r="A22" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M22" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="N22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="R22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="S22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="T22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="U22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="W22" s="29" t="s">
         <v>13</v>
       </c>
       <c r="X22" s="7">

</xml_diff>